<commit_message>
we can get the info correctly out of the excel files
</commit_message>
<xml_diff>
--- a/Anime BookmarkList.xlsx
+++ b/Anime BookmarkList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a10d998fb4a25b16/4docs/Coding/Java/AnimeBookmarkList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="178" documentId="8_{C6460328-8127-4B69-A488-9FAEB23349CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{358B494E-9E6E-4D5E-836C-31A8B8051B7F}"/>
+  <xr:revisionPtr revIDLastSave="181" documentId="8_{C6460328-8127-4B69-A488-9FAEB23349CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8F242D32-F429-4743-8086-8B041BC10553}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{F0FA748D-AA9F-4D99-B4E9-7C72EE416517}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="849" uniqueCount="296">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="296">
   <si>
     <t>11eyes</t>
   </si>
@@ -1320,8 +1320,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C32B5591-E57E-48C4-8308-44338EF9FD71}">
   <dimension ref="A1:C286"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
-      <selection activeCell="A290" sqref="A287:XFD290"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C88" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1489,6 +1489,9 @@
       <c r="A15" s="9" t="s">
         <v>289</v>
       </c>
+      <c r="C15" s="9" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1660,6 +1663,9 @@
         <v>294</v>
       </c>
       <c r="B31" s="8"/>
+      <c r="C31" s="7" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
@@ -2282,6 +2288,9 @@
         <v>295</v>
       </c>
       <c r="B88" s="12"/>
+      <c r="C88" s="11" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">

</xml_diff>